<commit_message>
Inclusión del README, migración de pip + env -> uv, eliminación de código innecesario
</commit_message>
<xml_diff>
--- a/docs_iniciales/prueba.xlsx
+++ b/docs_iniciales/prueba.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{564F41E0-5813-4ECD-BBF4-BF08FE283E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD4A8176-0224-4D3F-B477-6A3B85BA5CDE}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="936" yWindow="936" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" r:id="rId1"/>
@@ -2347,8 +2347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11913,8 +11913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6210E59-6336-4579-B845-2C53A07A6408}">
   <dimension ref="A1:A45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D16:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>